<commit_message>
Change iris data to penguin data
</commit_message>
<xml_diff>
--- a/gptables/test/test_additional_formatting_gptable.xlsx
+++ b/gptables/test/test_additional_formatting_gptable.xlsx
@@ -294,52 +294,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" indent="2" wrapText="1"/>
+      <alignment horizontal="left" indent="2" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" indent="2" wrapText="1"/>
+      <alignment horizontal="left" indent="2" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" indent="2" wrapText="1"/>
+      <alignment horizontal="left" indent="2" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" indent="2" wrapText="1"/>
+      <alignment horizontal="left" indent="2" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -759,7 +762,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -779,19 +782,19 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5">
         <v>3.758666666666666</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="10">
         <v>1.464</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="10">
         <v>4.26</v>
       </c>
       <c r="F9" s="5">
@@ -799,7 +802,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -808,10 +811,10 @@
       <c r="C10" s="5">
         <v>4.35</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="10">
         <v>1.5</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="10">
         <v>4.35</v>
       </c>
       <c r="F10" s="5">
@@ -819,27 +822,27 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="12">
         <v>1.198666666666667</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="13">
         <v>0.244</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="13">
         <v>1.326</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="12">
         <v>2.026</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -848,10 +851,10 @@
       <c r="C12" s="5">
         <v>1.3</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="10">
         <v>0.2</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="10">
         <v>1.3</v>
       </c>
       <c r="F12" s="5">
@@ -859,27 +862,27 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="15">
         <v>5.843333333333334</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="16">
         <v>5.006</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="16">
         <v>5.936</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="15">
         <v>6.587999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -888,10 +891,10 @@
       <c r="C14" s="5">
         <v>5.8</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="10">
         <v>5</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="10">
         <v>5.9</v>
       </c>
       <c r="F14" s="5">
@@ -899,7 +902,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -908,10 +911,10 @@
       <c r="C15" s="5">
         <v>3.054</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="10">
         <v>3.418</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="10">
         <v>2.77</v>
       </c>
       <c r="F15" s="5">
@@ -919,22 +922,22 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="18">
         <v>3</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="19">
         <v>3.4</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="19">
         <v>2.8</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="18">
         <v>3</v>
       </c>
     </row>

</xml_diff>